<commit_message>
5/22 update - FK upload working, more work to do
</commit_message>
<xml_diff>
--- a/misc/codes_test.xlsx
+++ b/misc/codes_test.xlsx
@@ -22,12 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t xml:space="preserve">code_id</t>
   </si>
   <si>
     <t xml:space="preserve">code_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">job</t>
   </si>
   <si>
     <t xml:space="preserve">footage</t>
@@ -396,20 +399,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E65536"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -424,6 +427,9 @@
       </c>
       <c r="E1" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,7 +437,10 @@
         <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,7 +448,10 @@
         <v>140</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -447,7 +459,10 @@
         <v>150</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +470,10 @@
         <v>160</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,7 +481,10 @@
         <v>178</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,7 +492,10 @@
         <v>220</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,7 +503,10 @@
         <v>230</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,7 +514,10 @@
         <v>240</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,7 +525,10 @@
         <v>250</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,7 +536,10 @@
         <v>260</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -511,7 +547,10 @@
         <v>320</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,7 +558,10 @@
         <v>330</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,7 +569,10 @@
         <v>340</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,7 +580,10 @@
         <v>350</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,7 +591,10 @@
         <v>360</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,7 +602,10 @@
         <v>420</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,7 +613,10 @@
         <v>430</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,7 +624,10 @@
         <v>440</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,7 +635,10 @@
         <v>450</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,7 +646,10 @@
         <v>460</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +657,10 @@
         <v>520</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,7 +668,10 @@
         <v>530</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,7 +679,10 @@
         <v>540</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -615,7 +690,10 @@
         <v>550</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,7 +701,10 @@
         <v>560</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +712,10 @@
         <v>7410</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,7 +723,10 @@
         <v>7415</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,7 +734,10 @@
         <v>7420</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -655,7 +745,10 @@
         <v>7425</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,7 +756,10 @@
         <v>7435</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,7 +767,10 @@
         <v>7496</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,7 +778,10 @@
         <v>7497</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,7 +789,10 @@
         <v>9720</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,7 +800,10 @@
         <v>7600</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,7 +811,10 @@
         <v>9047</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,7 +822,10 @@
         <v>9060</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,7 +833,10 @@
         <v>7101</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,7 +844,10 @@
         <v>170</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -735,7 +855,10 @@
         <v>210</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,7 +866,10 @@
         <v>270</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,7 +877,10 @@
         <v>282</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,7 +888,10 @@
         <v>310</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,7 +899,10 @@
         <v>370</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,7 +910,10 @@
         <v>382</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,7 +921,10 @@
         <v>410</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,7 +932,10 @@
         <v>470</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -799,7 +943,10 @@
         <v>482</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,7 +954,10 @@
         <v>510</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,7 +965,10 @@
         <v>570</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,7 +976,10 @@
         <v>582</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,7 +987,10 @@
         <v>7400</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,7 +998,10 @@
         <v>7405</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -868,7 +1030,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -894,7 +1056,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>